<commit_message>
Fix analytics API errors and remove duplicate offer details
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF17"/>
+  <dimension ref="A1:AF19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -646,7 +646,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>In Process</t>
+          <t>Rejected</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -703,7 +703,7 @@
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>{"Communication":"good ","Technical Assessment":"good","Problem-Solving":"","Overall Potential":"","Recommendation":""}</t>
+          <t>{"Communication":"good ","Technical Assessment":"good","Problem-Solving":"","Overall Potential":"","Recommendation":"Proceed Round 2"}</t>
         </is>
       </c>
       <c r="AB2" t="inlineStr">
@@ -2522,6 +2522,226 @@
       <c r="AE17" t="inlineStr"/>
       <c r="AF17" t="inlineStr"/>
     </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>JAGADEESH M</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>jagadeesh19ct11@gmail.com</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>06381813711</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Site Reliability Engineer</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Data Engineer</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>nill</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Coimbatore</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>400000</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>0-1 years</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Immediate</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>Rejected</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>Coimbatore</t>
+        </is>
+      </c>
+      <c r="V18" t="inlineStr">
+        <is>
+          <t>nill</t>
+        </is>
+      </c>
+      <c r="W18" t="inlineStr"/>
+      <c r="X18" t="inlineStr"/>
+      <c r="Y18" t="inlineStr"/>
+      <c r="Z18" t="inlineStr"/>
+      <c r="AA18" t="inlineStr"/>
+      <c r="AB18" t="inlineStr"/>
+      <c r="AC18" t="inlineStr"/>
+      <c r="AD18" t="inlineStr"/>
+      <c r="AE18" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AF18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>ashwin</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>ashlog559@gmail.com</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>0123456789</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Senior Site Reliability Engineer</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Senior Software Engineer</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>nill</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Chennai</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>100000000</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>999999999999998</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>2-3 years</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Immediate</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>Rejected</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>999999999999</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>Others</t>
+        </is>
+      </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>nill</t>
+        </is>
+      </c>
+      <c r="W19" t="inlineStr"/>
+      <c r="X19" t="inlineStr"/>
+      <c r="Y19" t="inlineStr"/>
+      <c r="Z19" t="inlineStr"/>
+      <c r="AA19" t="inlineStr"/>
+      <c r="AB19" t="inlineStr"/>
+      <c r="AC19" t="inlineStr"/>
+      <c r="AD19" t="inlineStr"/>
+      <c r="AE19" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="AF19" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix UI issues: remove duplicate Offer Details and enable Add New Candidate button
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -2349,12 +2349,12 @@
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>All Completed</t>
+          <t>Offer</t>
         </is>
       </c>
       <c r="N16" t="inlineStr">
         <is>
-          <t>Joined</t>
+          <t>In Notice</t>
         </is>
       </c>
       <c r="O16" t="inlineStr">
@@ -2479,13 +2479,17 @@
         </is>
       </c>
       <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="Q17" t="inlineStr"/>
       <c r="R17" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -2502,7 +2506,11 @@
           <t>Any</t>
         </is>
       </c>
-      <c r="V17" t="inlineStr"/>
+      <c r="V17" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
       <c r="W17" t="inlineStr">
         <is>
           <t>https://drive.google.com/file/d/1Wc0kEJXvwgeygTxVo8L0PBmr36_dgyoU/view?usp=drive_link</t>
@@ -2513,14 +2521,22 @@
           <t>https://www.linkedin.com/in/vishva-m/</t>
         </is>
       </c>
-      <c r="Y17" t="inlineStr"/>
+      <c r="Y17" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
       <c r="Z17" t="inlineStr"/>
       <c r="AA17" t="inlineStr"/>
       <c r="AB17" t="inlineStr"/>
       <c r="AC17" t="inlineStr"/>
       <c r="AD17" t="inlineStr"/>
       <c r="AE17" t="inlineStr"/>
-      <c r="AF17" t="inlineStr"/>
+      <c r="AF17" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
@@ -2627,13 +2643,17 @@
       <c r="AD18" t="inlineStr"/>
       <c r="AE18" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="AF18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr"/>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Invalid Date</t>
+        </is>
+      </c>
       <c r="B19" t="inlineStr">
         <is>
           <t>ashwin</t>
@@ -2684,34 +2704,34 @@
           <t>2-3 years</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>Immediate</t>
-        </is>
-      </c>
+      <c r="L19" t="inlineStr"/>
       <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr">
         <is>
           <t>Rejected</t>
         </is>
       </c>
-      <c r="O19" t="inlineStr"/>
-      <c r="P19" t="inlineStr"/>
-      <c r="Q19" t="inlineStr">
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="R19" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="S19" t="inlineStr">
-        <is>
-          <t>Yes</t>
-        </is>
-      </c>
       <c r="T19" t="inlineStr">
         <is>
           <t>999999999999</t>
@@ -2727,9 +2747,17 @@
           <t>nill</t>
         </is>
       </c>
-      <c r="W19" t="inlineStr"/>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
       <c r="X19" t="inlineStr"/>
-      <c r="Y19" t="inlineStr"/>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
       <c r="Z19" t="inlineStr"/>
       <c r="AA19" t="inlineStr"/>
       <c r="AB19" t="inlineStr"/>
@@ -2740,7 +2768,11 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="AF19" t="inlineStr"/>
+      <c r="AF19" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fix UI: Add missing AddModal, remove all Offer Details from index, fix caching
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -2293,7 +2293,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>2025-11-07 00:00:00</t>
+          <t>11/7/2025</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -2367,11 +2367,7 @@
           <t>Got to know about Guhatek from a friend Hussain Mahuvawala, Found the opportunity interesting hence applied.</t>
         </is>
       </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr">
         <is>
           <t>No</t>
@@ -2403,14 +2399,22 @@
           <t>https://www.linkedin.com/in/deepak-kayande-9612b739/</t>
         </is>
       </c>
-      <c r="Y16" t="inlineStr"/>
+      <c r="Y16" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
       <c r="Z16" t="inlineStr"/>
       <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="inlineStr"/>
       <c r="AC16" t="inlineStr"/>
       <c r="AD16" t="inlineStr"/>
       <c r="AE16" t="inlineStr"/>
-      <c r="AF16" t="inlineStr"/>
+      <c r="AF16" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2539,7 +2543,11 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr"/>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Invalid Date</t>
+        </is>
+      </c>
       <c r="B18" t="inlineStr">
         <is>
           <t>JAGADEESH M</t>
@@ -2590,24 +2598,24 @@
           <t>0-1 years</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>Immediate</t>
-        </is>
-      </c>
+      <c r="L18" t="inlineStr"/>
       <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr">
         <is>
           <t>Rejected</t>
         </is>
       </c>
-      <c r="O18" t="inlineStr"/>
-      <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr"/>
       <c r="R18" t="inlineStr">
         <is>
           <t>Yes</t>
@@ -2633,9 +2641,17 @@
           <t>nill</t>
         </is>
       </c>
-      <c r="W18" t="inlineStr"/>
+      <c r="W18" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
       <c r="X18" t="inlineStr"/>
-      <c r="Y18" t="inlineStr"/>
+      <c r="Y18" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
       <c r="Z18" t="inlineStr"/>
       <c r="AA18" t="inlineStr"/>
       <c r="AB18" t="inlineStr"/>
@@ -2646,7 +2662,11 @@
           <t>No</t>
         </is>
       </c>
-      <c r="AF18" t="inlineStr"/>
+      <c r="AF18" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">

</xml_diff>